<commit_message>
Tp2 cambiado a que ande
</commit_message>
<xml_diff>
--- a/resumen_promedios_actividades.xlsx
+++ b/resumen_promedios_actividades.xlsx
@@ -388,13 +388,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C2">
-        <v>4.142857142857143</v>
+        <v>4.224137931034483</v>
       </c>
       <c r="D2">
-        <v>4.14</v>
+        <v>4.22</v>
       </c>
     </row>
     <row r="3">
@@ -407,10 +407,10 @@
         <v>585</v>
       </c>
       <c r="C3">
-        <v>4.760683760683761</v>
+        <v>4.90940170940171</v>
       </c>
       <c r="D3">
-        <v>4.76</v>
+        <v>4.91</v>
       </c>
     </row>
     <row r="4">
@@ -423,10 +423,10 @@
         <v>481</v>
       </c>
       <c r="C4">
-        <v>4.952182952182953</v>
+        <v>5.014553014553014</v>
       </c>
       <c r="D4">
-        <v>4.95</v>
+        <v>5.01</v>
       </c>
     </row>
     <row r="5">
@@ -439,10 +439,10 @@
         <v>435</v>
       </c>
       <c r="C5">
-        <v>4.673563218390805</v>
+        <v>4.717241379310344</v>
       </c>
       <c r="D5">
-        <v>4.67</v>
+        <v>4.72</v>
       </c>
     </row>
     <row r="6">
@@ -455,10 +455,10 @@
         <v>92</v>
       </c>
       <c r="C6">
-        <v>4.391304347826087</v>
+        <v>4.434782608695652</v>
       </c>
       <c r="D6">
-        <v>4.39</v>
+        <v>4.43</v>
       </c>
     </row>
   </sheetData>
@@ -503,13 +503,13 @@
         </is>
       </c>
       <c r="B2">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="C2">
-        <v>4.776628748707342</v>
+        <v>4.863777089783282</v>
       </c>
       <c r="D2">
-        <v>4.78</v>
+        <v>4.86</v>
       </c>
     </row>
     <row r="3">
@@ -519,13 +519,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="C3">
-        <v>4.673441734417344</v>
+        <v>4.758108108108108</v>
       </c>
       <c r="D3">
-        <v>4.67</v>
+        <v>4.76</v>
       </c>
     </row>
   </sheetData>
@@ -573,10 +573,10 @@
         <v>422</v>
       </c>
       <c r="C2">
-        <v>4.928909952606635</v>
+        <v>5.014218009478673</v>
       </c>
       <c r="D2">
-        <v>4.93</v>
+        <v>5.01</v>
       </c>
     </row>
     <row r="3">
@@ -589,10 +589,10 @@
         <v>744</v>
       </c>
       <c r="C3">
-        <v>4.80241935483871</v>
+        <v>4.893817204301075</v>
       </c>
       <c r="D3">
-        <v>4.8</v>
+        <v>4.89</v>
       </c>
     </row>
     <row r="4">
@@ -605,42 +605,42 @@
         <v>122</v>
       </c>
       <c r="C4">
-        <v>4.598360655737705</v>
+        <v>4.647540983606557</v>
       </c>
       <c r="D4">
-        <v>4.6</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E.Jubilado</t>
+          <t>D.Estudiante</t>
         </is>
       </c>
       <c r="B5">
-        <v>120</v>
+        <v>272</v>
       </c>
       <c r="C5">
-        <v>4.475</v>
+        <v>4.544117647058823</v>
       </c>
       <c r="D5">
-        <v>4.47</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>D.Estudiante</t>
+          <t>E.Jubilado</t>
         </is>
       </c>
       <c r="B6">
-        <v>268</v>
+        <v>120</v>
       </c>
       <c r="C6">
-        <v>4.440298507462686</v>
+        <v>4.525</v>
       </c>
       <c r="D6">
-        <v>4.44</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="7">
@@ -653,10 +653,10 @@
         <v>29</v>
       </c>
       <c r="C7">
-        <v>4.379310344827586</v>
+        <v>4.517241379310345</v>
       </c>
       <c r="D7">
-        <v>4.38</v>
+        <v>4.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>